<commit_message>
shifted to selenium, much less buggy now
</commit_message>
<xml_diff>
--- a/Tests.xlsx
+++ b/Tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\script stuff\buggy messaging bot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C19C8CC8-4ADE-47C6-8044-5B506E1F9495}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEDC5FE8-727A-4D86-A264-2BA817F20E70}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3072" yWindow="3072" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Name</t>
   </si>
@@ -29,9 +29,6 @@
   </si>
   <si>
     <t>Panel</t>
-  </si>
-  <si>
-    <t>desai the god</t>
   </si>
 </sst>
 </file>
@@ -355,7 +352,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
@@ -375,12 +372,8 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="13.2">
-      <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="1">
-        <v>9511879289</v>
-      </c>
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="13.2">

</xml_diff>

<commit_message>
message has emojis! :smiley_cat:
</commit_message>
<xml_diff>
--- a/Tests.xlsx
+++ b/Tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\script stuff\buggy messaging bot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEDC5FE8-727A-4D86-A264-2BA817F20E70}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B96293C1-3AC2-4CBE-BAA7-2CE9705CAE0A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3072" yWindow="3072" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Name</t>
   </si>
@@ -29,6 +29,9 @@
   </si>
   <si>
     <t>Panel</t>
+  </si>
+  <si>
+    <t>Rittmang</t>
   </si>
 </sst>
 </file>
@@ -349,11 +352,9 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
@@ -372,8 +373,12 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="13.2">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1">
+        <v>8452047071</v>
+      </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="13.2">
@@ -396,6 +401,54 @@
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
     </row>
+    <row r="7" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+    </row>
+    <row r="8" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+    </row>
+    <row r="9" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+    </row>
+    <row r="10" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+    </row>
+    <row r="11" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+    </row>
+    <row r="12" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+    </row>
+    <row r="13" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+    </row>
+    <row r="14" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+    </row>
+    <row r="15" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+    </row>
+    <row r="16" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+    </row>
+    <row r="17" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+    </row>
+    <row r="18" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
just put message in one string, format in sendMessage and emojize
</commit_message>
<xml_diff>
--- a/Tests.xlsx
+++ b/Tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\script stuff\buggy messaging bot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B96293C1-3AC2-4CBE-BAA7-2CE9705CAE0A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35A3C7C9-8C64-4FF9-90D8-7A2A4AC36116}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3072" yWindow="3072" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -354,7 +354,9 @@
   </sheetPr>
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>

</xml_diff>

<commit_message>
waiting for important elements to load before performing action
</commit_message>
<xml_diff>
--- a/Tests.xlsx
+++ b/Tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\script stuff\buggy messaging bot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35A3C7C9-8C64-4FF9-90D8-7A2A4AC36116}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67B8CDEE-13E9-4787-A522-F7120B4F8011}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3072" yWindow="3072" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
     <t>Panel</t>
   </si>
   <si>
-    <t>Rittmang</t>
+    <t>Akhil</t>
   </si>
 </sst>
 </file>
@@ -355,7 +355,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
@@ -379,7 +379,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="1">
-        <v>8452047071</v>
+        <v>9921164006</v>
       </c>
       <c r="C2" s="1"/>
     </row>

</xml_diff>